<commit_message>
Update configuration tracking spreadsheet for project execution
Updates ConfigTracker2.xlsx.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: dce5354f-2436-410a-aa06-2c5c987da9b6
Replit-Commit-Checkpoint-Type: full_checkpoint
</commit_message>
<xml_diff>
--- a/ConfigTracker2.xlsx
+++ b/ConfigTracker2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub Repositories\ExcelToAPI_SampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3AA91D-87D3-469A-9671-70E9A888B6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666C22DA-90BA-4228-89E4-424598E54E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0A95F42-B9FA-4697-81E7-8A75D2048534}"/>
   </bookViews>
@@ -80,6 +80,9 @@
     <t>NAD</t>
   </si>
   <si>
+    <t>fireDomain.install</t>
+  </si>
+  <si>
     <t>fireDomain.insall.expense</t>
   </si>
   <si>
@@ -90,9 +93,6 @@
   </si>
   <si>
     <t>action</t>
-  </si>
-  <si>
-    <t>fireDomain.insall</t>
   </si>
   <si>
     <t>transactionDefaultAttributeValues</t>
@@ -488,7 +488,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -550,7 +550,7 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -567,7 +567,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -576,10 +576,10 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -619,7 +619,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -631,7 +631,7 @@
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update configuration tracker spreadsheet with latest information
Updated ConfigTracker2.xlsx file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: dce5354f-2436-410a-aa06-2c5c987da9b6
Replit-Commit-Checkpoint-Type: full_checkpoint
</commit_message>
<xml_diff>
--- a/ConfigTracker2.xlsx
+++ b/ConfigTracker2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub Repositories\ExcelToAPI_SampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666C22DA-90BA-4228-89E4-424598E54E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865BDA02-6545-45B4-A5F6-9E9C95990F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0A95F42-B9FA-4697-81E7-8A75D2048534}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>fireDomain.install</t>
   </si>
   <si>
-    <t>fireDomain.insall.expense</t>
-  </si>
-  <si>
     <t>serviceContractType</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>installLineAction</t>
+  </si>
+  <si>
+    <t>fireDomain.install.expense</t>
   </si>
 </sst>
 </file>
@@ -487,9 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374FC121-0482-44DB-ADB8-78963DA1593E}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -541,7 +539,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -550,7 +548,7 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -567,7 +565,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -576,10 +574,10 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -602,7 +600,7 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -628,10 +626,10 @@
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update configuration tracking with new item categories
Update ConfigTracker2.xlsx to include Configuration, Commerce, and Document Designer item types.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: dce5354f-2436-410a-aa06-2c5c987da9b6
Replit-Commit-Checkpoint-Type: full_checkpoint
</commit_message>
<xml_diff>
--- a/ConfigTracker2.xlsx
+++ b/ConfigTracker2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub Repositories\ExcelToAPI_SampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865BDA02-6545-45B4-A5F6-9E9C95990F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E8737E-A091-40CD-BF23-02417B1AACBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0A95F42-B9FA-4697-81E7-8A75D2048534}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>itemName</t>
   </si>
@@ -99,16 +99,55 @@
   </si>
   <si>
     <t>fireDomain.install.expense</t>
+  </si>
+  <si>
+    <t>Commerce</t>
+  </si>
+  <si>
+    <t>oraclecpqo_bmClone_2</t>
+  </si>
+  <si>
+    <t>transaction</t>
+  </si>
+  <si>
+    <t>aPI_Save_t</t>
+  </si>
+  <si>
+    <t>save_start_step</t>
+  </si>
+  <si>
+    <t>oraclecpqo_bmClone_3</t>
+  </si>
+  <si>
+    <t>NAD-10759</t>
+  </si>
+  <si>
+    <t>Archana</t>
+  </si>
+  <si>
+    <t>Document Designer</t>
+  </si>
+  <si>
+    <t>Hybrid Quote Document Design - English</t>
+  </si>
+  <si>
+    <t>doc_designer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,13 +203,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,13 +525,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374FC121-0482-44DB-ADB8-78963DA1593E}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="36.140625" customWidth="1"/>
@@ -529,110 +569,192 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="b">
+      <c r="E2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="b">
+      <c r="E3" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="b">
+      <c r="E4" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="b">
+      <c r="E5" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="6" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6" xr:uid="{46E04E21-9F7F-4477-99EA-771EB79F2172}">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>